<commit_message>
Milestones, Time and Effort Matrix
</commit_message>
<xml_diff>
--- a/Time_Effort_Milestone.xlsx
+++ b/Time_Effort_Milestone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Fall 2024\CS5001 - Senior Design 1\Euchre-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C08C98-B0C3-432D-9466-D92603E1E443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0570730F-4576-417E-904C-0124CD99DC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:XFD31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>